<commit_message>
Add report for cook
</commit_message>
<xml_diff>
--- a/reports/report_20250613.xlsx
+++ b/reports/report_20250613.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -40,6 +40,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFD966"/>
         <bgColor rgb="00FFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCFFCC"/>
+        <bgColor rgb="00CCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,7 +67,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -69,6 +75,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +451,7 @@
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
     <col width="6" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -472,7 +479,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -481,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Шашлык Баранина</t>
+          <t>Шашлык Утка</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -489,8 +496,60 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Шашлык Баранина</t>
+        </is>
+      </c>
       <c r="D3" t="n">
         <v>1900</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Шашлык Утка - Шашлык Баранина - Кока Кола2л</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr"/>
+      <c r="B6" s="3" t="inlineStr"/>
+      <c r="C6" s="3" t="inlineStr"/>
+      <c r="D6" s="3" t="n">
+        <v>9400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>